<commit_message>
Changes to final datasets
</commit_message>
<xml_diff>
--- a/distribution_palette.xlsx
+++ b/distribution_palette.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\4th Year\4th Year Courses\STA 474 2.0 Statistical Consultancy\Project 1 - Visualizing Examination Timetable\Examination-Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,15 +16,15 @@
   </sheets>
   <calcPr calcId="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Alphabetical order" guid="{EDEC074E-F25A-4530-B103-55BB375C7831}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{FB50271F-8772-4DCE-927B-BB257CA92E03}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{BF19D836-2735-42D9-9519-7B8517737261}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{FB50271F-8772-4DCE-927B-BB257CA92E03}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Alphabetical order" guid="{EDEC074E-F25A-4530-B103-55BB375C7831}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
   <si>
     <t>Subject</t>
   </si>
@@ -212,13 +212,19 @@
   </si>
   <si>
     <t>#9500e6</t>
+  </si>
+  <si>
+    <t>PBT</t>
+  </si>
+  <si>
+    <t>#dede5d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -242,8 +248,22 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="31">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +444,12 @@
         <bgColor rgb="FFE600E5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEDE5D"/>
+        <bgColor rgb="FFDCDC89"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -575,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -650,6 +676,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,6 +688,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDEDE5D"/>
       <color rgb="FF9500E6"/>
     </mruColors>
   </colors>
@@ -873,10 +904,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1103,7 +1134,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="49.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>36</v>
       </c>
@@ -1116,153 +1147,160 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="49.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="44"/>
+      <c r="C18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="49.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="1" t="s">
+      <c r="B19" s="31"/>
+      <c r="C19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D19" s="16" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="49.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="49.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="32"/>
+      <c r="C20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="49.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="42" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D21" s="29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="49.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+    <row r="22" spans="1:4" ht="49.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="13" t="s">
+      <c r="B22" s="33"/>
+      <c r="C22" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D22" s="16" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="35"/>
+        <v>44</v>
+      </c>
+      <c r="B23" s="34"/>
       <c r="C23" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="35"/>
+      <c r="C24" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="21" t="s">
+      <c r="B25" s="36"/>
+      <c r="C25" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+    <row r="26" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="37"/>
-      <c r="C25" s="5" t="s">
+      <c r="B26" s="37"/>
+      <c r="C26" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
+    <row r="27" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="13" t="s">
+      <c r="B27" s="38"/>
+      <c r="C27" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D27" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="5" t="s">
+      <c r="B28" s="39"/>
+      <c r="C28" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
+    <row r="29" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="13" t="s">
+      <c r="B29" s="40"/>
+      <c r="C29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D29" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="9" t="s">
+      <c r="B30" s="41"/>
+      <c r="C30" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D30" s="9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
@@ -6129,7 +6167,13 @@
       <c r="C1003" s="2"/>
       <c r="D1003" s="2"/>
     </row>
+    <row r="1004" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1004" s="2"/>
+      <c r="C1004" s="2"/>
+      <c r="D1004" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>